<commit_message>
6 features baseline beaten
</commit_message>
<xml_diff>
--- a/6_Final_projects/1_user_identification/kaggle/results.xlsx
+++ b/6_Final_projects/1_user_identification/kaggle/results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16692075\Git\Specialization-Yandex-MIPT\6_Final_projects\1_user_identification\kaggle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Git\Uniholder\Specialization-Yandex-MIPT\6_Final_projects\1_user_identification\kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675D947-64AB-47FD-989E-49AE5E3063CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="28995" windowHeight="15675" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="111">
   <si>
     <t>model</t>
   </si>
@@ -316,12 +317,54 @@
   </si>
   <si>
     <t>0.94882</t>
+  </si>
+  <si>
+    <t>hour_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9327937119878204 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9349913447341495 </t>
+  </si>
+  <si>
+    <t>0.95034</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9353851373113711 </t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9369922517305278 </t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9373161534312052 </t>
+  </si>
+  <si>
+    <t>0.95257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9375198540384677 </t>
+  </si>
+  <si>
+    <t>session_duration</t>
+  </si>
+  <si>
+    <t>0.95319</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -384,15 +427,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,7 +468,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-FD9D0B08863FD7EBB1D3FC206A5503EF/1.png"/>
+        <xdr:cNvPr id="4" name="Рисунок 3" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-FD9D0B08863FD7EBB1D3FC206A5503EF/1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -467,7 +517,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-FD9D0B08863FD7EBB1D3FC206A5503EF/1.png"/>
+        <xdr:cNvPr id="3" name="Рисунок 2" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-FD9D0B08863FD7EBB1D3FC206A5503EF/1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -755,29 +811,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A8:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3984375" customWidth="1"/>
+    <col min="8" max="8" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:9" x14ac:dyDescent="0.45">
       <c r="H8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,7 +850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E10" t="s">
         <v>3</v>
       </c>
@@ -807,18 +863,18 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="6" t="s">
+    <row r="11" spans="5:9" x14ac:dyDescent="0.45">
+      <c r="E11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
@@ -832,7 +888,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
@@ -840,7 +896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
@@ -848,7 +904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E15" t="s">
         <v>3</v>
       </c>
@@ -862,7 +918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E16" t="s">
         <v>3</v>
       </c>
@@ -876,7 +932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E17" t="s">
         <v>3</v>
       </c>
@@ -890,7 +946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E18" t="s">
         <v>38</v>
       </c>
@@ -902,7 +958,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E19" t="s">
         <v>39</v>
       </c>
@@ -916,7 +972,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E20" t="s">
         <v>39</v>
       </c>
@@ -930,7 +986,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -941,7 +997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>18</v>
       </c>
@@ -949,7 +1005,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E23" t="s">
         <v>3</v>
       </c>
@@ -963,7 +1019,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E24" t="s">
         <v>3</v>
       </c>
@@ -977,7 +1033,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E25" t="s">
         <v>3</v>
       </c>
@@ -989,7 +1045,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E26" t="s">
         <v>3</v>
       </c>
@@ -1003,7 +1059,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E27" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1073,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E28" t="s">
         <v>3</v>
       </c>
@@ -1033,11 +1089,8 @@
       <c r="I28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E29" s="1" t="s">
         <v>20</v>
       </c>
@@ -1045,19 +1098,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E30" s="1"/>
+      <c r="H30" t="s">
+        <v>106</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E31" s="1" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1072,301 +1137,618 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:T20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A7:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="9.140625" style="7"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="7"/>
-    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="7"/>
-    <col min="17" max="17" width="11.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="7"/>
-    <col min="19" max="19" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="7"/>
+    <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="6"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="6" max="9" width="9.1328125" style="6"/>
+    <col min="11" max="11" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.265625" customWidth="1"/>
+    <col min="14" max="14" width="6" style="6" customWidth="1"/>
+    <col min="15" max="15" width="10.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1328125" style="6"/>
+    <col min="17" max="17" width="11.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1328125" style="6"/>
+    <col min="19" max="19" width="13.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1328125" style="6"/>
+    <col min="22" max="22" width="14.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="L7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="M7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="N7" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="O7" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="S7" s="7" t="s">
+      <c r="Q7" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="R7" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A8" s="6"/>
+      <c r="B8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="C8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+      <c r="C9"/>
+      <c r="D9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A10" s="6"/>
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="C10"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A11" s="6"/>
+      <c r="B11" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="C11"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A12" s="6"/>
+      <c r="B12" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="C12"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A13" s="6"/>
+      <c r="B13" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M13" s="7" t="s">
+      <c r="C13"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A14" s="6"/>
+      <c r="B14" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M14" s="7" t="s">
+      <c r="C14"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="K14" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A15" s="6"/>
+      <c r="B15" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M15" s="7" t="s">
+      <c r="C15"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="K15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="L15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A16" s="6"/>
+      <c r="B16" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M16" s="7" t="s">
+      <c r="C16"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="K16" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="O16" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="L16" s="6"/>
+      <c r="M16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A17" s="6"/>
+      <c r="B17" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" s="7" t="s">
+      <c r="C17"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="K17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="P17" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A18" s="6"/>
+      <c r="B18" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="C18"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="K18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Q18" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="O18" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B19" t="s">
         <v>93</v>
       </c>
-      <c r="E19" t="s">
+      <c r="C19" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="7" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="K19" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="R19" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="P19" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A20" s="6"/>
+      <c r="B20" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M20" s="7" t="s">
+      <c r="C20"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="K20" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="S20" s="7" t="s">
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="Q20" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A21" s="6"/>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="K21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="P21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="K22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="K23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="K24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="K25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="K26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="V26" s="6" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A3 baseline (10 credits) beaten
</commit_message>
<xml_diff>
--- a/6_Final_projects/1_user_identification/kaggle/results.xlsx
+++ b/6_Final_projects/1_user_identification/kaggle/results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16692075\Git\Specialization-Yandex-MIPT\6_Final_projects\1_user_identification\kaggle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Git\Uniholder\Specialization-Yandex-MIPT\6_Final_projects\1_user_identification\kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C8E6D-E46E-49B7-B162-8096F385644D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="28995" windowHeight="15675" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="128">
   <si>
     <t>model</t>
   </si>
@@ -174,9 +175,6 @@
     <t>0.94310</t>
   </si>
   <si>
-    <t>!</t>
-  </si>
-  <si>
     <t>bag of sites; CountVectorizer (1, 2)-grams 20k; morning, day, evening, night, weekday, duration, year_month</t>
   </si>
   <si>
@@ -385,12 +383,39 @@
   </si>
   <si>
     <t>overfitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.937618123149331 </t>
+  </si>
+  <si>
+    <t>7_unique</t>
+  </si>
+  <si>
+    <t>0.95340</t>
+  </si>
+  <si>
+    <t>0.94876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9144307686524599 </t>
+  </si>
+  <si>
+    <t>balanced</t>
+  </si>
+  <si>
+    <t>0.95766</t>
+  </si>
+  <si>
+    <t>0.9375190037899295</t>
+  </si>
+  <si>
+    <t>{'alpha': 3.6e-05, 'penalty': 'l2'}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -463,14 +488,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -502,7 +530,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-7500C9C76CEBFA3E4567AC715FAEBEC2/1.png"/>
+        <xdr:cNvPr id="2" name="Рисунок 1" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-7500C9C76CEBFA3E4567AC715FAEBEC2/1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -545,7 +579,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-7500C9C76CEBFA3E4567AC715FAEBEC2/1.png"/>
+        <xdr:cNvPr id="2" name="Рисунок 1" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-7500C9C76CEBFA3E4567AC715FAEBEC2/1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -833,29 +873,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:J32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A8:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3984375" customWidth="1"/>
+    <col min="8" max="8" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3984375" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:9" x14ac:dyDescent="0.45">
       <c r="H8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E9" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E10" t="s">
         <v>3</v>
       </c>
@@ -885,18 +925,18 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="8" t="s">
+    <row r="11" spans="5:9" x14ac:dyDescent="0.45">
+      <c r="E11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
@@ -910,7 +950,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
@@ -918,7 +958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
@@ -926,7 +966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E15" t="s">
         <v>3</v>
       </c>
@@ -940,7 +980,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E16" t="s">
         <v>3</v>
       </c>
@@ -954,7 +994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E17" t="s">
         <v>3</v>
       </c>
@@ -968,7 +1008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E18" t="s">
         <v>38</v>
       </c>
@@ -980,7 +1020,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E19" t="s">
         <v>39</v>
       </c>
@@ -994,7 +1034,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E20" t="s">
         <v>39</v>
       </c>
@@ -1008,7 +1048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1019,7 +1059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1027,7 +1067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E23" t="s">
         <v>3</v>
       </c>
@@ -1041,78 +1081,78 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E24" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" t="s">
         <v>50</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E25" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" t="s">
         <v>53</v>
       </c>
-      <c r="H25" t="s">
-        <v>54</v>
-      </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E26" t="s">
         <v>3</v>
       </c>
       <c r="F26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s">
         <v>55</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="E27" t="s">
         <v>3</v>
       </c>
       <c r="F27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" t="s">
         <v>58</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="E28" t="s">
         <v>3</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G28" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E29" s="1" t="s">
         <v>20</v>
       </c>
@@ -1120,19 +1160,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E30" s="1"/>
       <c r="H30" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>22</v>
       </c>
@@ -1140,11 +1177,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="1" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E32" s="1"/>
+      <c r="H32" t="s">
+        <v>126</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.45">
+      <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1159,119 +1205,130 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:Y29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A7:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="6"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1328125" style="6"/>
+    <col min="8" max="8" width="7.53125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.19921875" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.06640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A7" s="6"/>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="H7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="K7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="Q7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="X7" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="X7" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="Y7" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" s="6"/>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8"/>
       <c r="D8" s="6"/>
@@ -1281,14 +1338,14 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" s="6"/>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9"/>
       <c r="D9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="6"/>
       <c r="H9"/>
@@ -1296,631 +1353,772 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" s="6"/>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" s="6"/>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" s="6"/>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" s="6"/>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" s="6"/>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
       <c r="K14" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" s="6"/>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
       <c r="K15" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
       <c r="K16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17" s="6"/>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
       <c r="K17" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18" s="6"/>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
       <c r="K18" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="O18" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
       <c r="K19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="P19" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A20" s="6"/>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
       <c r="K20" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="Q20" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A21" s="6"/>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="K21" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="P21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
       <c r="K22" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
       <c r="K23" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
       <c r="K24" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="K25" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U25" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="K26" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V26" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
       <c r="K27" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W27" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
       <c r="K28" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V28" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X28" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>118</v>
-      </c>
       <c r="E29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="K29" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y29" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="K30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="U30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="V30" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z30" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="K31" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z31" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA31" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="K32" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="U32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="V32" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z32" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>